<commit_message>
Updated summary_classification_report with logistic regression patient-known-features results.
</commit_message>
<xml_diff>
--- a/Data/summary_classification_report.xlsx
+++ b/Data/summary_classification_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cam Foster\Documents\Education\Georgia Tech\Homework\FinalProject\final-project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965AA6FB-7948-4328-BDC4-9C9B86EACCFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B636C8-B3B0-4E9F-94F9-E54395BA3A62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{505989D8-F08E-4569-892A-A8D9A00AD870}"/>
+    <workbookView xWindow="4800" yWindow="2115" windowWidth="18420" windowHeight="11055" activeTab="1" xr2:uid="{505989D8-F08E-4569-892A-A8D9A00AD870}"/>
   </bookViews>
   <sheets>
     <sheet name="all-features" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,6 +671,18 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
+      <c r="B6">
+        <v>0.67</v>
+      </c>
+      <c r="C6">
+        <v>0.61</v>
+      </c>
+      <c r="D6">
+        <v>0.61</v>
+      </c>
+      <c r="E6">
+        <v>0.51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added summary_classification_report with scaled numbers.
</commit_message>
<xml_diff>
--- a/Data/summary_classification_report.xlsx
+++ b/Data/summary_classification_report.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cam Foster\Documents\Education\Georgia Tech\Homework\FinalProject\final-project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591D759C-7A4D-4235-8503-72C3D7B61671}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFC81F1-D4FA-42F6-9488-3831C6A29308}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="2250" windowWidth="18420" windowHeight="11055" xr2:uid="{505989D8-F08E-4569-892A-A8D9A00AD870}"/>
+    <workbookView xWindow="-23025" yWindow="2850" windowWidth="18420" windowHeight="11055" firstSheet="1" activeTab="3" xr2:uid="{505989D8-F08E-4569-892A-A8D9A00AD870}"/>
   </bookViews>
   <sheets>
-    <sheet name="all-features" sheetId="1" r:id="rId1"/>
-    <sheet name="patient-known-features" sheetId="3" r:id="rId2"/>
+    <sheet name="patient-known-features" sheetId="5" r:id="rId1"/>
+    <sheet name="all-features" sheetId="4" r:id="rId2"/>
+    <sheet name="all-features_source" sheetId="1" r:id="rId3"/>
+    <sheet name="patient-known-features_source" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
   <si>
     <t>model</t>
   </si>
@@ -515,11 +517,300 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DFA6F5-1D6F-4222-9317-06ED80328B5A}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8">
+        <f>'patient-known-features_source'!B2/MAX('patient-known-features_source'!B$2:B$6)</f>
+        <v>0.91994572591587453</v>
+      </c>
+      <c r="C2" s="8">
+        <f>'patient-known-features_source'!C2/MAX('patient-known-features_source'!C$2:C$6)</f>
+        <v>0.97619047619047583</v>
+      </c>
+      <c r="D2" s="8">
+        <f>'patient-known-features_source'!D2/MAX('patient-known-features_source'!D$2:D$6)</f>
+        <v>0.97619047619047583</v>
+      </c>
+      <c r="E2" s="8">
+        <f>'patient-known-features_source'!E2/MAX('patient-known-features_source'!E$2:E$6)</f>
+        <v>0.9343659179755619</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8">
+        <f>'patient-known-features_source'!B3/MAX('patient-known-features_source'!B$2:B$6)</f>
+        <v>0.96236210253082377</v>
+      </c>
+      <c r="C3" s="8">
+        <f>'patient-known-features_source'!C3/MAX('patient-known-features_source'!C$2:C$6)</f>
+        <v>0.91428571428571437</v>
+      </c>
+      <c r="D3" s="8">
+        <f>'patient-known-features_source'!D3/MAX('patient-known-features_source'!D$2:D$6)</f>
+        <v>0.91428571428571437</v>
+      </c>
+      <c r="E3" s="8">
+        <f>'patient-known-features_source'!E3/MAX('patient-known-features_source'!E$2:E$6)</f>
+        <v>0.97572494139376242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8">
+        <f>'patient-known-features_source'!B4/MAX('patient-known-features_source'!B$2:B$6)</f>
+        <v>0.90909090909090895</v>
+      </c>
+      <c r="C4" s="8">
+        <f>'patient-known-features_source'!C4/MAX('patient-known-features_source'!C$2:C$6)</f>
+        <v>0.92857142857142871</v>
+      </c>
+      <c r="D4" s="8">
+        <f>'patient-known-features_source'!D4/MAX('patient-known-features_source'!D$2:D$6)</f>
+        <v>0.92857142857142871</v>
+      </c>
+      <c r="E4" s="8">
+        <f>'patient-known-features_source'!E4/MAX('patient-known-features_source'!E$2:E$6)</f>
+        <v>0.94372331487165317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8">
+        <f>'patient-known-features_source'!B5/MAX('patient-known-features_source'!B$2:B$6)</f>
+        <v>0.98737083811710591</v>
+      </c>
+      <c r="C5" s="8">
+        <f>'patient-known-features_source'!C5/MAX('patient-known-features_source'!C$2:C$6)</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="8">
+        <f>'patient-known-features_source'!D5/MAX('patient-known-features_source'!D$2:D$6)</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
+        <f>'patient-known-features_source'!E5/MAX('patient-known-features_source'!E$2:E$6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8">
+        <f>'patient-known-features_source'!B6/MAX('patient-known-features_source'!B$2:B$6)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <f>'patient-known-features_source'!C6/MAX('patient-known-features_source'!C$2:C$6)</f>
+        <v>0.87142857142857144</v>
+      </c>
+      <c r="D6" s="8">
+        <f>'patient-known-features_source'!D6/MAX('patient-known-features_source'!D$2:D$6)</f>
+        <v>0.87142857142857144</v>
+      </c>
+      <c r="E6" s="8">
+        <f>'patient-known-features_source'!E6/MAX('patient-known-features_source'!E$2:E$6)</f>
+        <v>0.77476379910492288</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEBAC9C-22EE-4C2D-A1D3-4E4380C41F32}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8">
+        <f>'all-features_source'!B2/MAX('all-features_source'!B$2:B$6)</f>
+        <v>0.93035130718954251</v>
+      </c>
+      <c r="C2" s="8">
+        <f>'all-features_source'!C2/MAX('all-features_source'!C$2:C$6)</f>
+        <v>0.94514767932489363</v>
+      </c>
+      <c r="D2" s="8">
+        <f>'all-features_source'!D2/MAX('all-features_source'!D$2:D$6)</f>
+        <v>0.94514767932489363</v>
+      </c>
+      <c r="E2" s="8">
+        <f>'all-features_source'!E2/MAX('all-features_source'!E$2:E$6)</f>
+        <v>0.95555866418666924</v>
+      </c>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8">
+        <f>'all-features_source'!B3/MAX('all-features_source'!B$2:B$6)</f>
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="C3" s="8">
+        <f>'all-features_source'!C3/MAX('all-features_source'!C$2:C$6)</f>
+        <v>0.97890295358649737</v>
+      </c>
+      <c r="D3" s="8">
+        <f>'all-features_source'!D3/MAX('all-features_source'!D$2:D$6)</f>
+        <v>0.97890295358649737</v>
+      </c>
+      <c r="E3" s="8">
+        <f>'all-features_source'!E3/MAX('all-features_source'!E$2:E$6)</f>
+        <v>0.99701468122520764</v>
+      </c>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8">
+        <f>'all-features_source'!B4/MAX('all-features_source'!B$2:B$6)</f>
+        <v>0.74239417989417988</v>
+      </c>
+      <c r="C4" s="8">
+        <f>'all-features_source'!C4/MAX('all-features_source'!C$2:C$6)</f>
+        <v>0.810126582278481</v>
+      </c>
+      <c r="D4" s="8">
+        <f>'all-features_source'!D4/MAX('all-features_source'!D$2:D$6)</f>
+        <v>0.810126582278481</v>
+      </c>
+      <c r="E4" s="8">
+        <f>'all-features_source'!E4/MAX('all-features_source'!E$2:E$6)</f>
+        <v>0.76598041199811029</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8">
+        <f>'all-features_source'!B5/MAX('all-features_source'!B$2:B$6)</f>
+        <v>0.91118292205248619</v>
+      </c>
+      <c r="C5" s="8">
+        <f>'all-features_source'!C5/MAX('all-features_source'!C$2:C$6)</f>
+        <v>0.90717299578058985</v>
+      </c>
+      <c r="D5" s="8">
+        <f>'all-features_source'!D5/MAX('all-features_source'!D$2:D$6)</f>
+        <v>0.90717299578058985</v>
+      </c>
+      <c r="E5" s="8">
+        <f>'all-features_source'!E5/MAX('all-features_source'!E$2:E$6)</f>
+        <v>0.92439859881720254</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8">
+        <f>'all-features_source'!B6/MAX('all-features_source'!B$2:B$6)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <f>'all-features_source'!C6/MAX('all-features_source'!C$2:C$6)</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <f>'all-features_source'!D6/MAX('all-features_source'!D$2:D$6)</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <f>'all-features_source'!E6/MAX('all-features_source'!E$2:E$6)</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A655E0-4001-4B6B-B311-B56785349F02}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,12 +927,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3306D3-45C9-4924-AB93-E604CA79320B}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="A1:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>